<commit_message>
Historia, enemigos y sonidos
Se ha completado la historia, se han colocado todos los enemigos y se han puesto todos los sonidos.
</commit_message>
<xml_diff>
--- a/TacticalTakedown/Mapas.xlsx
+++ b/TacticalTakedown/Mapas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Documents\GitHub\IngenieBROS\TacticalTakedown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60095E8A-8292-4880-99D1-C3ABB2EA4ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A2E4F1-0F85-430F-92C6-A1CBAC6D7F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8F948029-4BD6-4DEB-B888-1B838FCC9D45}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{8F948029-4BD6-4DEB-B888-1B838FCC9D45}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -817,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0119C222-3848-4BEA-BDB4-7D06439B5ED9}">
   <dimension ref="B1:BD111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D69" sqref="D69:Z98"/>
     </sheetView>
   </sheetViews>
@@ -1094,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="6">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="L5" s="6">
         <v>1</v>
@@ -1112,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="Q5" s="6">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="R5" s="6">
         <v>1</v>
@@ -1349,10 +1349,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="6">
+        <v>35</v>
+      </c>
+      <c r="G8" s="6">
         <v>32</v>
-      </c>
-      <c r="G8" s="6">
-        <v>35</v>
       </c>
       <c r="H8" s="8">
         <v>18</v>
@@ -1580,7 +1580,7 @@
         <v>18</v>
       </c>
       <c r="W10" s="6">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="X10" s="6">
         <v>34</v>
@@ -2030,7 +2030,7 @@
         <v>18</v>
       </c>
       <c r="W15" s="6">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="X15" s="6">
         <v>34</v>
@@ -3902,7 +3902,7 @@
         <v>1</v>
       </c>
       <c r="N38" s="6">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="O38" s="6">
         <v>1</v>
@@ -4272,7 +4272,7 @@
         <v>34</v>
       </c>
       <c r="G43" s="6">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H43" s="6">
         <v>18</v>
@@ -4462,10 +4462,10 @@
         <v>25</v>
       </c>
       <c r="W45" s="6">
+        <v>33</v>
+      </c>
+      <c r="X45" s="6">
         <v>35</v>
-      </c>
-      <c r="X45" s="6">
-        <v>33</v>
       </c>
       <c r="Y45" s="6">
         <v>1</v>
@@ -6017,7 +6017,7 @@
         <v>1</v>
       </c>
       <c r="O70" s="5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P70" s="8">
         <v>1</v>
@@ -6097,7 +6097,7 @@
         <v>1</v>
       </c>
       <c r="O71" s="5">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P71" s="5">
         <v>1</v>
@@ -6393,7 +6393,7 @@
         <v>34</v>
       </c>
       <c r="G75" s="6">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H75" s="6">
         <v>18</v>
@@ -6441,7 +6441,7 @@
         <v>18</v>
       </c>
       <c r="W75" s="6">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="X75" s="6">
         <v>34</v>
@@ -6873,7 +6873,7 @@
         <v>34</v>
       </c>
       <c r="G81" s="6">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H81" s="6">
         <v>18</v>
@@ -6921,7 +6921,7 @@
         <v>18</v>
       </c>
       <c r="W81" s="6">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="X81" s="6">
         <v>34</v>
@@ -7353,7 +7353,7 @@
         <v>34</v>
       </c>
       <c r="G87" s="6">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H87" s="6">
         <v>18</v>
@@ -7401,7 +7401,7 @@
         <v>18</v>
       </c>
       <c r="W87" s="6">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="X87" s="6">
         <v>34</v>
@@ -7833,7 +7833,7 @@
         <v>34</v>
       </c>
       <c r="G93" s="6">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H93" s="6">
         <v>18</v>
@@ -7881,7 +7881,7 @@
         <v>18</v>
       </c>
       <c r="W93" s="6">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="X93" s="6">
         <v>34</v>

</xml_diff>